<commit_message>
SMBExcel: Write new constructor, new tests TestSMBExcel: Add few new tests;
</commit_message>
<xml_diff>
--- a/Patterns/pattern1.xlsx
+++ b/Patterns/pattern1.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>test</t>
+    <t>Text in cell A1</t>
   </si>
 </sst>
 </file>
@@ -359,11 +359,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Add following properties: ActiveWorksheet and Field (without code yet) Add tests for those properties
</commit_message>
<xml_diff>
--- a/Patterns/pattern1.xlsx
+++ b/Patterns/pattern1.xlsx
@@ -16,9 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Text in cell A1</t>
+  </si>
+  <si>
+    <t>#Param1</t>
   </si>
 </sst>
 </file>
@@ -357,18 +360,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Move class methods to new class TestSMBExcelClassMembers. Add to class TSMBExcel: 1. property Range 2. Methods Show and Hide 3. Method Copy
</commit_message>
<xml_diff>
--- a/Patterns/pattern1.xlsx
+++ b/Patterns/pattern1.xlsx
@@ -11,24 +11,40 @@
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <definedNames>
+    <definedName name="RangeA10B11">Лист1!$A$10:$B$11</definedName>
+    <definedName name="RangeE7">Лист1!$E$7</definedName>
+  </definedNames>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Text in cell A1</t>
   </si>
   <si>
     <t>#Param1</t>
   </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>B10</t>
+  </si>
+  <si>
+    <t>B11</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00&quot;р.&quot;_-;\-* #,##0.00&quot;р.&quot;_-;_-* &quot;-&quot;??&quot;р.&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -36,16 +52,54 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -53,14 +107,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Денежный" xfId="1" builtinId="4"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -360,25 +436,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A10" sqref="A10:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="1">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <f>10+3</f>
+        <v>13</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>